<commit_message>
PP & test plan update
</commit_message>
<xml_diff>
--- a/Testing/Group1 Test Case Plan.xlsx
+++ b/Testing/Group1 Test Case Plan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Scenario</t>
   </si>
@@ -98,9 +98,6 @@
     <t>TestNormalPARAGRP</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Test adding a Sensor to a start trigger and one to a stop trigger. Test ability to toggle a Sensor on and off</t>
   </si>
   <si>
@@ -159,6 +156,12 @@
   </si>
   <si>
     <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>Testing specific error, not 'real' error</t>
+  </si>
+  <si>
+    <t>Printing error</t>
   </si>
 </sst>
 </file>
@@ -550,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J14"/>
+  <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +602,7 @@
     </row>
     <row r="2" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -619,13 +622,13 @@
     </row>
     <row r="3" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -634,7 +637,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>17</v>
@@ -642,7 +645,7 @@
     </row>
     <row r="4" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -662,7 +665,7 @@
     </row>
     <row r="5" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -677,7 +680,7 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>19</v>
@@ -685,10 +688,10 @@
     </row>
     <row r="6" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -699,16 +702,16 @@
     </row>
     <row r="7" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -716,13 +719,13 @@
     </row>
     <row r="8" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
         <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -733,51 +736,55 @@
         <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
         <v>36</v>
       </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="28.8" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:10" ht="28.8" x14ac:dyDescent="0.3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>